<commit_message>
modified and final framework
</commit_message>
<xml_diff>
--- a/ActiTime-AutomationLevel-4/Controller/data_Controller.xlsx
+++ b/ActiTime-AutomationLevel-4/Controller/data_Controller.xlsx
@@ -97,9 +97,6 @@
     <t>launchBrowser--&gt;navigate --&gt; Login--&gt;CreateCustomer--&gt;CreateProject--&gt;ModifyProject--&gt;DeleteProject--&gt;DeleteCustomer--&gt;logout--&gt;closeApplication</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>TC08</t>
   </si>
   <si>
@@ -107,6 +104,9 @@
   </si>
   <si>
     <t>launchBrowser--&gt;navigate --&gt; Login--&gt;CreateCustomer--&gt;CreateProject--&gt;CreateTask--&gt;DeleteTask--&gt;DeleteCustomer--&gt;logout--&gt;closeApplication</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -464,7 +464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -500,7 +500,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -514,7 +514,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -528,7 +528,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -542,7 +542,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -556,7 +556,7 @@
         <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -570,7 +570,7 @@
         <v>21</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -584,21 +584,21 @@
         <v>24</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="D9" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>